<commit_message>
Got team defensive stats working too
</commit_message>
<xml_diff>
--- a/data/NFL_2024_team.xlsx
+++ b/data/NFL_2024_team.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Offensive_team_stats" sheetId="1" r:id="rId1"/>
+    <sheet name="Defensive_team_stats" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="621">
   <si>
     <t>Rk</t>
   </si>
@@ -1874,6 +1875,9 @@
   </si>
   <si>
     <t>66.7</t>
+  </si>
+  <si>
+    <t>PA</t>
   </si>
 </sst>
 </file>
@@ -5426,4 +5430,3194 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AC36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:29">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2">
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <v>301</v>
+      </c>
+      <c r="F2">
+        <v>5514</v>
+      </c>
+      <c r="G2">
+        <v>1037</v>
+      </c>
+      <c r="H2">
+        <v>5.3</v>
+      </c>
+      <c r="I2">
+        <v>21</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+      <c r="K2">
+        <v>311</v>
+      </c>
+      <c r="L2">
+        <v>367</v>
+      </c>
+      <c r="M2">
+        <v>565</v>
+      </c>
+      <c r="N2">
+        <v>3517</v>
+      </c>
+      <c r="O2">
+        <v>24</v>
+      </c>
+      <c r="P2">
+        <v>15</v>
+      </c>
+      <c r="Q2">
+        <v>5.8</v>
+      </c>
+      <c r="R2">
+        <v>170</v>
+      </c>
+      <c r="S2">
+        <v>426</v>
+      </c>
+      <c r="T2">
+        <v>1997</v>
+      </c>
+      <c r="U2">
+        <v>7</v>
+      </c>
+      <c r="V2">
+        <v>4.7</v>
+      </c>
+      <c r="W2">
+        <v>108</v>
+      </c>
+      <c r="X2">
+        <v>101</v>
+      </c>
+      <c r="Y2">
+        <v>869</v>
+      </c>
+      <c r="Z2">
+        <v>33</v>
+      </c>
+      <c r="AA2">
+        <v>32.6</v>
+      </c>
+      <c r="AB2">
+        <v>11.6</v>
+      </c>
+      <c r="AC2">
+        <v>-12.31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3">
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <v>303</v>
+      </c>
+      <c r="F3">
+        <v>4732</v>
+      </c>
+      <c r="G3">
+        <v>999</v>
+      </c>
+      <c r="H3">
+        <v>4.7</v>
+      </c>
+      <c r="I3">
+        <v>26</v>
+      </c>
+      <c r="J3">
+        <v>13</v>
+      </c>
+      <c r="K3">
+        <v>293</v>
+      </c>
+      <c r="L3">
+        <v>337</v>
+      </c>
+      <c r="M3">
+        <v>542</v>
+      </c>
+      <c r="N3">
+        <v>2961</v>
+      </c>
+      <c r="O3">
+        <v>22</v>
+      </c>
+      <c r="P3">
+        <v>13</v>
+      </c>
+      <c r="Q3">
+        <v>5.1</v>
+      </c>
+      <c r="R3">
+        <v>160</v>
+      </c>
+      <c r="S3">
+        <v>416</v>
+      </c>
+      <c r="T3">
+        <v>1771</v>
+      </c>
+      <c r="U3">
+        <v>9</v>
+      </c>
+      <c r="V3">
+        <v>4.3</v>
+      </c>
+      <c r="W3">
+        <v>108</v>
+      </c>
+      <c r="X3">
+        <v>85</v>
+      </c>
+      <c r="Y3">
+        <v>694</v>
+      </c>
+      <c r="Z3">
+        <v>25</v>
+      </c>
+      <c r="AA3">
+        <v>31.6</v>
+      </c>
+      <c r="AB3">
+        <v>14.1</v>
+      </c>
+      <c r="AC3">
+        <v>76.38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <v>311</v>
+      </c>
+      <c r="F4">
+        <v>5391</v>
+      </c>
+      <c r="G4">
+        <v>1093</v>
+      </c>
+      <c r="H4">
+        <v>4.9</v>
+      </c>
+      <c r="I4">
+        <v>25</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>327</v>
+      </c>
+      <c r="L4">
+        <v>393</v>
+      </c>
+      <c r="M4">
+        <v>606</v>
+      </c>
+      <c r="N4">
+        <v>3752</v>
+      </c>
+      <c r="O4">
+        <v>22</v>
+      </c>
+      <c r="P4">
+        <v>15</v>
+      </c>
+      <c r="Q4">
+        <v>5.6</v>
+      </c>
+      <c r="R4">
+        <v>203</v>
+      </c>
+      <c r="S4">
+        <v>424</v>
+      </c>
+      <c r="T4">
+        <v>1639</v>
+      </c>
+      <c r="U4">
+        <v>10</v>
+      </c>
+      <c r="V4">
+        <v>3.9</v>
+      </c>
+      <c r="W4">
+        <v>82</v>
+      </c>
+      <c r="X4">
+        <v>101</v>
+      </c>
+      <c r="Y4">
+        <v>723</v>
+      </c>
+      <c r="Z4">
+        <v>42</v>
+      </c>
+      <c r="AA4">
+        <v>31.6</v>
+      </c>
+      <c r="AB4">
+        <v>12.4</v>
+      </c>
+      <c r="AC4">
+        <v>34.83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>326</v>
+      </c>
+      <c r="F5">
+        <v>5451</v>
+      </c>
+      <c r="G5">
+        <v>1026</v>
+      </c>
+      <c r="H5">
+        <v>5.3</v>
+      </c>
+      <c r="I5">
+        <v>20</v>
+      </c>
+      <c r="J5">
+        <v>7</v>
+      </c>
+      <c r="K5">
+        <v>328</v>
+      </c>
+      <c r="L5">
+        <v>375</v>
+      </c>
+      <c r="M5">
+        <v>569</v>
+      </c>
+      <c r="N5">
+        <v>3720</v>
+      </c>
+      <c r="O5">
+        <v>24</v>
+      </c>
+      <c r="P5">
+        <v>13</v>
+      </c>
+      <c r="Q5">
+        <v>6.1</v>
+      </c>
+      <c r="R5">
+        <v>191</v>
+      </c>
+      <c r="S5">
+        <v>418</v>
+      </c>
+      <c r="T5">
+        <v>1731</v>
+      </c>
+      <c r="U5">
+        <v>13</v>
+      </c>
+      <c r="V5">
+        <v>4.1</v>
+      </c>
+      <c r="W5">
+        <v>112</v>
+      </c>
+      <c r="X5">
+        <v>107</v>
+      </c>
+      <c r="Y5">
+        <v>849</v>
+      </c>
+      <c r="Z5">
+        <v>25</v>
+      </c>
+      <c r="AA5">
+        <v>36.5</v>
+      </c>
+      <c r="AB5">
+        <v>11.4</v>
+      </c>
+      <c r="AC5">
+        <v>-74.11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6">
+        <v>17</v>
+      </c>
+      <c r="E6">
+        <v>332</v>
+      </c>
+      <c r="F6">
+        <v>5702</v>
+      </c>
+      <c r="G6">
+        <v>1078</v>
+      </c>
+      <c r="H6">
+        <v>5.3</v>
+      </c>
+      <c r="I6">
+        <v>33</v>
+      </c>
+      <c r="J6">
+        <v>9</v>
+      </c>
+      <c r="K6">
+        <v>325</v>
+      </c>
+      <c r="L6">
+        <v>415</v>
+      </c>
+      <c r="M6">
+        <v>637</v>
+      </c>
+      <c r="N6">
+        <v>4114</v>
+      </c>
+      <c r="O6">
+        <v>24</v>
+      </c>
+      <c r="P6">
+        <v>24</v>
+      </c>
+      <c r="Q6">
+        <v>6</v>
+      </c>
+      <c r="R6">
+        <v>218</v>
+      </c>
+      <c r="S6">
+        <v>392</v>
+      </c>
+      <c r="T6">
+        <v>1588</v>
+      </c>
+      <c r="U6">
+        <v>12</v>
+      </c>
+      <c r="V6">
+        <v>4.1</v>
+      </c>
+      <c r="W6">
+        <v>83</v>
+      </c>
+      <c r="X6">
+        <v>141</v>
+      </c>
+      <c r="Y6">
+        <v>1185</v>
+      </c>
+      <c r="Z6">
+        <v>24</v>
+      </c>
+      <c r="AA6">
+        <v>31.6</v>
+      </c>
+      <c r="AB6">
+        <v>16.6</v>
+      </c>
+      <c r="AC6">
+        <v>35.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>338</v>
+      </c>
+      <c r="F7">
+        <v>5347</v>
+      </c>
+      <c r="G7">
+        <v>1036</v>
+      </c>
+      <c r="H7">
+        <v>5.2</v>
+      </c>
+      <c r="I7">
+        <v>31</v>
+      </c>
+      <c r="J7">
+        <v>14</v>
+      </c>
+      <c r="K7">
+        <v>327</v>
+      </c>
+      <c r="L7">
+        <v>381</v>
+      </c>
+      <c r="M7">
+        <v>565</v>
+      </c>
+      <c r="N7">
+        <v>3658</v>
+      </c>
+      <c r="O7">
+        <v>23</v>
+      </c>
+      <c r="P7">
+        <v>17</v>
+      </c>
+      <c r="Q7">
+        <v>6</v>
+      </c>
+      <c r="R7">
+        <v>200</v>
+      </c>
+      <c r="S7">
+        <v>426</v>
+      </c>
+      <c r="T7">
+        <v>1689</v>
+      </c>
+      <c r="U7">
+        <v>13</v>
+      </c>
+      <c r="V7">
+        <v>4</v>
+      </c>
+      <c r="W7">
+        <v>104</v>
+      </c>
+      <c r="X7">
+        <v>114</v>
+      </c>
+      <c r="Y7">
+        <v>940</v>
+      </c>
+      <c r="Z7">
+        <v>23</v>
+      </c>
+      <c r="AA7">
+        <v>33</v>
+      </c>
+      <c r="AB7">
+        <v>16.2</v>
+      </c>
+      <c r="AC7">
+        <v>10.82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8">
+        <v>17</v>
+      </c>
+      <c r="E8">
+        <v>342</v>
+      </c>
+      <c r="F8">
+        <v>5820</v>
+      </c>
+      <c r="G8">
+        <v>1016</v>
+      </c>
+      <c r="H8">
+        <v>5.7</v>
+      </c>
+      <c r="I8">
+        <v>24</v>
+      </c>
+      <c r="J8">
+        <v>8</v>
+      </c>
+      <c r="K8">
+        <v>331</v>
+      </c>
+      <c r="L8">
+        <v>373</v>
+      </c>
+      <c r="M8">
+        <v>610</v>
+      </c>
+      <c r="N8">
+        <v>4148</v>
+      </c>
+      <c r="O8">
+        <v>18</v>
+      </c>
+      <c r="P8">
+        <v>16</v>
+      </c>
+      <c r="Q8">
+        <v>6.4</v>
+      </c>
+      <c r="R8">
+        <v>198</v>
+      </c>
+      <c r="S8">
+        <v>369</v>
+      </c>
+      <c r="T8">
+        <v>1672</v>
+      </c>
+      <c r="U8">
+        <v>18</v>
+      </c>
+      <c r="V8">
+        <v>4.5</v>
+      </c>
+      <c r="W8">
+        <v>86</v>
+      </c>
+      <c r="X8">
+        <v>114</v>
+      </c>
+      <c r="Y8">
+        <v>862</v>
+      </c>
+      <c r="Z8">
+        <v>47</v>
+      </c>
+      <c r="AA8">
+        <v>35.4</v>
+      </c>
+      <c r="AB8">
+        <v>13.3</v>
+      </c>
+      <c r="AC8">
+        <v>-58.06</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>347</v>
+      </c>
+      <c r="F9">
+        <v>5554</v>
+      </c>
+      <c r="G9">
+        <v>1034</v>
+      </c>
+      <c r="H9">
+        <v>5.4</v>
+      </c>
+      <c r="I9">
+        <v>33</v>
+      </c>
+      <c r="J9">
+        <v>16</v>
+      </c>
+      <c r="K9">
+        <v>324</v>
+      </c>
+      <c r="L9">
+        <v>382</v>
+      </c>
+      <c r="M9">
+        <v>582</v>
+      </c>
+      <c r="N9">
+        <v>3876</v>
+      </c>
+      <c r="O9">
+        <v>23</v>
+      </c>
+      <c r="P9">
+        <v>17</v>
+      </c>
+      <c r="Q9">
+        <v>6.2</v>
+      </c>
+      <c r="R9">
+        <v>193</v>
+      </c>
+      <c r="S9">
+        <v>412</v>
+      </c>
+      <c r="T9">
+        <v>1678</v>
+      </c>
+      <c r="U9">
+        <v>14</v>
+      </c>
+      <c r="V9">
+        <v>4.1</v>
+      </c>
+      <c r="W9">
+        <v>108</v>
+      </c>
+      <c r="X9">
+        <v>125</v>
+      </c>
+      <c r="Y9">
+        <v>1039</v>
+      </c>
+      <c r="Z9">
+        <v>23</v>
+      </c>
+      <c r="AA9">
+        <v>34.6</v>
+      </c>
+      <c r="AB9">
+        <v>15.9</v>
+      </c>
+      <c r="AC9">
+        <v>-34.89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>361</v>
+      </c>
+      <c r="F10">
+        <v>5511</v>
+      </c>
+      <c r="G10">
+        <v>1062</v>
+      </c>
+      <c r="H10">
+        <v>5.2</v>
+      </c>
+      <c r="I10">
+        <v>17</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
+      <c r="K10">
+        <v>330</v>
+      </c>
+      <c r="L10">
+        <v>396</v>
+      </c>
+      <c r="M10">
+        <v>625</v>
+      </c>
+      <c r="N10">
+        <v>4150</v>
+      </c>
+      <c r="O10">
+        <v>27</v>
+      </c>
+      <c r="P10">
+        <v>12</v>
+      </c>
+      <c r="Q10">
+        <v>6.1</v>
+      </c>
+      <c r="R10">
+        <v>218</v>
+      </c>
+      <c r="S10">
+        <v>383</v>
+      </c>
+      <c r="T10">
+        <v>1361</v>
+      </c>
+      <c r="U10">
+        <v>12</v>
+      </c>
+      <c r="V10">
+        <v>3.6</v>
+      </c>
+      <c r="W10">
+        <v>69</v>
+      </c>
+      <c r="X10">
+        <v>97</v>
+      </c>
+      <c r="Y10">
+        <v>759</v>
+      </c>
+      <c r="Z10">
+        <v>43</v>
+      </c>
+      <c r="AA10">
+        <v>36.6</v>
+      </c>
+      <c r="AB10">
+        <v>9.1</v>
+      </c>
+      <c r="AC10">
+        <v>-49.44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11">
+        <v>17</v>
+      </c>
+      <c r="E11">
+        <v>364</v>
+      </c>
+      <c r="F11">
+        <v>5345</v>
+      </c>
+      <c r="G11">
+        <v>1012</v>
+      </c>
+      <c r="H11">
+        <v>5.3</v>
+      </c>
+      <c r="I11">
+        <v>16</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>314</v>
+      </c>
+      <c r="L11">
+        <v>365</v>
+      </c>
+      <c r="M11">
+        <v>572</v>
+      </c>
+      <c r="N11">
+        <v>3582</v>
+      </c>
+      <c r="O11">
+        <v>22</v>
+      </c>
+      <c r="P11">
+        <v>10</v>
+      </c>
+      <c r="Q11">
+        <v>5.9</v>
+      </c>
+      <c r="R11">
+        <v>190</v>
+      </c>
+      <c r="S11">
+        <v>405</v>
+      </c>
+      <c r="T11">
+        <v>1763</v>
+      </c>
+      <c r="U11">
+        <v>12</v>
+      </c>
+      <c r="V11">
+        <v>4.4</v>
+      </c>
+      <c r="W11">
+        <v>97</v>
+      </c>
+      <c r="X11">
+        <v>125</v>
+      </c>
+      <c r="Y11">
+        <v>1030</v>
+      </c>
+      <c r="Z11">
+        <v>27</v>
+      </c>
+      <c r="AA11">
+        <v>38.7</v>
+      </c>
+      <c r="AB11">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="AC11">
+        <v>-5.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12">
+        <v>17</v>
+      </c>
+      <c r="E12">
+        <v>368</v>
+      </c>
+      <c r="F12">
+        <v>5806</v>
+      </c>
+      <c r="G12">
+        <v>1052</v>
+      </c>
+      <c r="H12">
+        <v>5.5</v>
+      </c>
+      <c r="I12">
+        <v>32</v>
+      </c>
+      <c r="J12">
+        <v>16</v>
+      </c>
+      <c r="K12">
+        <v>356</v>
+      </c>
+      <c r="L12">
+        <v>396</v>
+      </c>
+      <c r="M12">
+        <v>578</v>
+      </c>
+      <c r="N12">
+        <v>3843</v>
+      </c>
+      <c r="O12">
+        <v>28</v>
+      </c>
+      <c r="P12">
+        <v>16</v>
+      </c>
+      <c r="Q12">
+        <v>6.2</v>
+      </c>
+      <c r="R12">
+        <v>217</v>
+      </c>
+      <c r="S12">
+        <v>435</v>
+      </c>
+      <c r="T12">
+        <v>1963</v>
+      </c>
+      <c r="U12">
+        <v>13</v>
+      </c>
+      <c r="V12">
+        <v>4.5</v>
+      </c>
+      <c r="W12">
+        <v>109</v>
+      </c>
+      <c r="X12">
+        <v>127</v>
+      </c>
+      <c r="Y12">
+        <v>1016</v>
+      </c>
+      <c r="Z12">
+        <v>30</v>
+      </c>
+      <c r="AA12">
+        <v>36.3</v>
+      </c>
+      <c r="AB12">
+        <v>17.5</v>
+      </c>
+      <c r="AC12">
+        <v>-76.45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13">
+        <v>17</v>
+      </c>
+      <c r="E13">
+        <v>368</v>
+      </c>
+      <c r="F13">
+        <v>5656</v>
+      </c>
+      <c r="G13">
+        <v>1065</v>
+      </c>
+      <c r="H13">
+        <v>5.3</v>
+      </c>
+      <c r="I13">
+        <v>18</v>
+      </c>
+      <c r="J13">
+        <v>5</v>
+      </c>
+      <c r="K13">
+        <v>329</v>
+      </c>
+      <c r="L13">
+        <v>371</v>
+      </c>
+      <c r="M13">
+        <v>569</v>
+      </c>
+      <c r="N13">
+        <v>3603</v>
+      </c>
+      <c r="O13">
+        <v>26</v>
+      </c>
+      <c r="P13">
+        <v>13</v>
+      </c>
+      <c r="Q13">
+        <v>5.9</v>
+      </c>
+      <c r="R13">
+        <v>193</v>
+      </c>
+      <c r="S13">
+        <v>451</v>
+      </c>
+      <c r="T13">
+        <v>2053</v>
+      </c>
+      <c r="U13">
+        <v>11</v>
+      </c>
+      <c r="V13">
+        <v>4.6</v>
+      </c>
+      <c r="W13">
+        <v>107</v>
+      </c>
+      <c r="X13">
+        <v>121</v>
+      </c>
+      <c r="Y13">
+        <v>958</v>
+      </c>
+      <c r="Z13">
+        <v>29</v>
+      </c>
+      <c r="AA13">
+        <v>34</v>
+      </c>
+      <c r="AB13">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="AC13">
+        <v>-11.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14">
+        <v>17</v>
+      </c>
+      <c r="E14">
+        <v>370</v>
+      </c>
+      <c r="F14">
+        <v>6022</v>
+      </c>
+      <c r="G14">
+        <v>1028</v>
+      </c>
+      <c r="H14">
+        <v>5.9</v>
+      </c>
+      <c r="I14">
+        <v>24</v>
+      </c>
+      <c r="J14">
+        <v>13</v>
+      </c>
+      <c r="K14">
+        <v>326</v>
+      </c>
+      <c r="L14">
+        <v>325</v>
+      </c>
+      <c r="M14">
+        <v>503</v>
+      </c>
+      <c r="N14">
+        <v>3705</v>
+      </c>
+      <c r="O14">
+        <v>17</v>
+      </c>
+      <c r="P14">
+        <v>11</v>
+      </c>
+      <c r="Q14">
+        <v>6.8</v>
+      </c>
+      <c r="R14">
+        <v>177</v>
+      </c>
+      <c r="S14">
+        <v>485</v>
+      </c>
+      <c r="T14">
+        <v>2317</v>
+      </c>
+      <c r="U14">
+        <v>20</v>
+      </c>
+      <c r="V14">
+        <v>4.8</v>
+      </c>
+      <c r="W14">
+        <v>129</v>
+      </c>
+      <c r="X14">
+        <v>107</v>
+      </c>
+      <c r="Y14">
+        <v>794</v>
+      </c>
+      <c r="Z14">
+        <v>20</v>
+      </c>
+      <c r="AA14">
+        <v>40.5</v>
+      </c>
+      <c r="AB14">
+        <v>13</v>
+      </c>
+      <c r="AC14">
+        <v>-53.66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15">
+        <v>17</v>
+      </c>
+      <c r="E15">
+        <v>372</v>
+      </c>
+      <c r="F15">
+        <v>5355</v>
+      </c>
+      <c r="G15">
+        <v>1050</v>
+      </c>
+      <c r="H15">
+        <v>5.1</v>
+      </c>
+      <c r="I15">
+        <v>29</v>
+      </c>
+      <c r="J15">
+        <v>10</v>
+      </c>
+      <c r="K15">
+        <v>313</v>
+      </c>
+      <c r="L15">
+        <v>326</v>
+      </c>
+      <c r="M15">
+        <v>554</v>
+      </c>
+      <c r="N15">
+        <v>3417</v>
+      </c>
+      <c r="O15">
+        <v>31</v>
+      </c>
+      <c r="P15">
+        <v>19</v>
+      </c>
+      <c r="Q15">
+        <v>5.7</v>
+      </c>
+      <c r="R15">
+        <v>172</v>
+      </c>
+      <c r="S15">
+        <v>447</v>
+      </c>
+      <c r="T15">
+        <v>1938</v>
+      </c>
+      <c r="U15">
+        <v>11</v>
+      </c>
+      <c r="V15">
+        <v>4.3</v>
+      </c>
+      <c r="W15">
+        <v>107</v>
+      </c>
+      <c r="X15">
+        <v>106</v>
+      </c>
+      <c r="Y15">
+        <v>798</v>
+      </c>
+      <c r="Z15">
+        <v>34</v>
+      </c>
+      <c r="AA15">
+        <v>35.2</v>
+      </c>
+      <c r="AB15">
+        <v>14</v>
+      </c>
+      <c r="AC15">
+        <v>20.49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16">
+        <v>17</v>
+      </c>
+      <c r="E16">
+        <v>379</v>
+      </c>
+      <c r="F16">
+        <v>5823</v>
+      </c>
+      <c r="G16">
+        <v>1045</v>
+      </c>
+      <c r="H16">
+        <v>5.6</v>
+      </c>
+      <c r="I16">
+        <v>17</v>
+      </c>
+      <c r="J16">
+        <v>8</v>
+      </c>
+      <c r="K16">
+        <v>344</v>
+      </c>
+      <c r="L16">
+        <v>370</v>
+      </c>
+      <c r="M16">
+        <v>539</v>
+      </c>
+      <c r="N16">
+        <v>3674</v>
+      </c>
+      <c r="O16">
+        <v>20</v>
+      </c>
+      <c r="P16">
+        <v>9</v>
+      </c>
+      <c r="Q16">
+        <v>6.3</v>
+      </c>
+      <c r="R16">
+        <v>200</v>
+      </c>
+      <c r="S16">
+        <v>465</v>
+      </c>
+      <c r="T16">
+        <v>2149</v>
+      </c>
+      <c r="U16">
+        <v>18</v>
+      </c>
+      <c r="V16">
+        <v>4.6</v>
+      </c>
+      <c r="W16">
+        <v>124</v>
+      </c>
+      <c r="X16">
+        <v>100</v>
+      </c>
+      <c r="Y16">
+        <v>803</v>
+      </c>
+      <c r="Z16">
+        <v>20</v>
+      </c>
+      <c r="AA16">
+        <v>43.1</v>
+      </c>
+      <c r="AB16">
+        <v>9.6</v>
+      </c>
+      <c r="AC16">
+        <v>-110.14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17">
+        <v>17</v>
+      </c>
+      <c r="E17">
+        <v>385</v>
+      </c>
+      <c r="F17">
+        <v>5810</v>
+      </c>
+      <c r="G17">
+        <v>1065</v>
+      </c>
+      <c r="H17">
+        <v>5.5</v>
+      </c>
+      <c r="I17">
+        <v>18</v>
+      </c>
+      <c r="J17">
+        <v>11</v>
+      </c>
+      <c r="K17">
+        <v>336</v>
+      </c>
+      <c r="L17">
+        <v>418</v>
+      </c>
+      <c r="M17">
+        <v>630</v>
+      </c>
+      <c r="N17">
+        <v>4147</v>
+      </c>
+      <c r="O17">
+        <v>27</v>
+      </c>
+      <c r="P17">
+        <v>7</v>
+      </c>
+      <c r="Q17">
+        <v>6.1</v>
+      </c>
+      <c r="R17">
+        <v>212</v>
+      </c>
+      <c r="S17">
+        <v>389</v>
+      </c>
+      <c r="T17">
+        <v>1663</v>
+      </c>
+      <c r="U17">
+        <v>13</v>
+      </c>
+      <c r="V17">
+        <v>4.3</v>
+      </c>
+      <c r="W17">
+        <v>94</v>
+      </c>
+      <c r="X17">
+        <v>96</v>
+      </c>
+      <c r="Y17">
+        <v>897</v>
+      </c>
+      <c r="Z17">
+        <v>30</v>
+      </c>
+      <c r="AA17">
+        <v>40.1</v>
+      </c>
+      <c r="AB17">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="AC17">
+        <v>-87.52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <v>386</v>
+      </c>
+      <c r="F18">
+        <v>6003</v>
+      </c>
+      <c r="G18">
+        <v>1057</v>
+      </c>
+      <c r="H18">
+        <v>5.7</v>
+      </c>
+      <c r="I18">
+        <v>20</v>
+      </c>
+      <c r="J18">
+        <v>7</v>
+      </c>
+      <c r="K18">
+        <v>342</v>
+      </c>
+      <c r="L18">
+        <v>354</v>
+      </c>
+      <c r="M18">
+        <v>542</v>
+      </c>
+      <c r="N18">
+        <v>3793</v>
+      </c>
+      <c r="O18">
+        <v>29</v>
+      </c>
+      <c r="P18">
+        <v>13</v>
+      </c>
+      <c r="Q18">
+        <v>6.5</v>
+      </c>
+      <c r="R18">
+        <v>196</v>
+      </c>
+      <c r="S18">
+        <v>477</v>
+      </c>
+      <c r="T18">
+        <v>2210</v>
+      </c>
+      <c r="U18">
+        <v>13</v>
+      </c>
+      <c r="V18">
+        <v>4.6</v>
+      </c>
+      <c r="W18">
+        <v>117</v>
+      </c>
+      <c r="X18">
+        <v>113</v>
+      </c>
+      <c r="Y18">
+        <v>948</v>
+      </c>
+      <c r="Z18">
+        <v>29</v>
+      </c>
+      <c r="AA18">
+        <v>42.9</v>
+      </c>
+      <c r="AB18">
+        <v>10.6</v>
+      </c>
+      <c r="AC18">
+        <v>-86.45999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19">
+        <v>17</v>
+      </c>
+      <c r="E19">
+        <v>391</v>
+      </c>
+      <c r="F19">
+        <v>5558</v>
+      </c>
+      <c r="G19">
+        <v>1029</v>
+      </c>
+      <c r="H19">
+        <v>5.4</v>
+      </c>
+      <c r="I19">
+        <v>17</v>
+      </c>
+      <c r="J19">
+        <v>10</v>
+      </c>
+      <c r="K19">
+        <v>335</v>
+      </c>
+      <c r="L19">
+        <v>307</v>
+      </c>
+      <c r="M19">
+        <v>496</v>
+      </c>
+      <c r="N19">
+        <v>3221</v>
+      </c>
+      <c r="O19">
+        <v>25</v>
+      </c>
+      <c r="P19">
+        <v>7</v>
+      </c>
+      <c r="Q19">
+        <v>6</v>
+      </c>
+      <c r="R19">
+        <v>175</v>
+      </c>
+      <c r="S19">
+        <v>490</v>
+      </c>
+      <c r="T19">
+        <v>2337</v>
+      </c>
+      <c r="U19">
+        <v>18</v>
+      </c>
+      <c r="V19">
+        <v>4.8</v>
+      </c>
+      <c r="W19">
+        <v>122</v>
+      </c>
+      <c r="X19">
+        <v>105</v>
+      </c>
+      <c r="Y19">
+        <v>849</v>
+      </c>
+      <c r="Z19">
+        <v>38</v>
+      </c>
+      <c r="AA19">
+        <v>41.5</v>
+      </c>
+      <c r="AB19">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="AC19">
+        <v>-147.39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20">
+        <v>17</v>
+      </c>
+      <c r="E20">
+        <v>398</v>
+      </c>
+      <c r="F20">
+        <v>6459</v>
+      </c>
+      <c r="G20">
+        <v>1119</v>
+      </c>
+      <c r="H20">
+        <v>5.8</v>
+      </c>
+      <c r="I20">
+        <v>17</v>
+      </c>
+      <c r="J20">
+        <v>3</v>
+      </c>
+      <c r="K20">
+        <v>354</v>
+      </c>
+      <c r="L20">
+        <v>366</v>
+      </c>
+      <c r="M20">
+        <v>591</v>
+      </c>
+      <c r="N20">
+        <v>4055</v>
+      </c>
+      <c r="O20">
+        <v>19</v>
+      </c>
+      <c r="P20">
+        <v>14</v>
+      </c>
+      <c r="Q20">
+        <v>6.4</v>
+      </c>
+      <c r="R20">
+        <v>194</v>
+      </c>
+      <c r="S20">
+        <v>489</v>
+      </c>
+      <c r="T20">
+        <v>2404</v>
+      </c>
+      <c r="U20">
+        <v>20</v>
+      </c>
+      <c r="V20">
+        <v>4.9</v>
+      </c>
+      <c r="W20">
+        <v>133</v>
+      </c>
+      <c r="X20">
+        <v>115</v>
+      </c>
+      <c r="Y20">
+        <v>959</v>
+      </c>
+      <c r="Z20">
+        <v>27</v>
+      </c>
+      <c r="AA20">
+        <v>39.3</v>
+      </c>
+      <c r="AB20">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="AC20">
+        <v>-107.32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21">
+        <v>17</v>
+      </c>
+      <c r="E21">
+        <v>404</v>
+      </c>
+      <c r="F21">
+        <v>5334</v>
+      </c>
+      <c r="G21">
+        <v>1068</v>
+      </c>
+      <c r="H21">
+        <v>5</v>
+      </c>
+      <c r="I21">
+        <v>17</v>
+      </c>
+      <c r="J21">
+        <v>10</v>
+      </c>
+      <c r="K21">
+        <v>347</v>
+      </c>
+      <c r="L21">
+        <v>327</v>
+      </c>
+      <c r="M21">
+        <v>521</v>
+      </c>
+      <c r="N21">
+        <v>3275</v>
+      </c>
+      <c r="O21">
+        <v>18</v>
+      </c>
+      <c r="P21">
+        <v>7</v>
+      </c>
+      <c r="Q21">
+        <v>5.8</v>
+      </c>
+      <c r="R21">
+        <v>171</v>
+      </c>
+      <c r="S21">
+        <v>504</v>
+      </c>
+      <c r="T21">
+        <v>2059</v>
+      </c>
+      <c r="U21">
+        <v>22</v>
+      </c>
+      <c r="V21">
+        <v>4.1</v>
+      </c>
+      <c r="W21">
+        <v>129</v>
+      </c>
+      <c r="X21">
+        <v>104</v>
+      </c>
+      <c r="Y21">
+        <v>989</v>
+      </c>
+      <c r="Z21">
+        <v>47</v>
+      </c>
+      <c r="AA21">
+        <v>44.6</v>
+      </c>
+      <c r="AB21">
+        <v>8.6</v>
+      </c>
+      <c r="AC21">
+        <v>-93.23999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22">
+        <v>17</v>
+      </c>
+      <c r="E22">
+        <v>415</v>
+      </c>
+      <c r="F22">
+        <v>5896</v>
+      </c>
+      <c r="G22">
+        <v>1051</v>
+      </c>
+      <c r="H22">
+        <v>5.6</v>
+      </c>
+      <c r="I22">
+        <v>15</v>
+      </c>
+      <c r="J22">
+        <v>10</v>
+      </c>
+      <c r="K22">
+        <v>331</v>
+      </c>
+      <c r="L22">
+        <v>349</v>
+      </c>
+      <c r="M22">
+        <v>503</v>
+      </c>
+      <c r="N22">
+        <v>3580</v>
+      </c>
+      <c r="O22">
+        <v>23</v>
+      </c>
+      <c r="P22">
+        <v>5</v>
+      </c>
+      <c r="Q22">
+        <v>6.5</v>
+      </c>
+      <c r="R22">
+        <v>177</v>
+      </c>
+      <c r="S22">
+        <v>503</v>
+      </c>
+      <c r="T22">
+        <v>2316</v>
+      </c>
+      <c r="U22">
+        <v>18</v>
+      </c>
+      <c r="V22">
+        <v>4.6</v>
+      </c>
+      <c r="W22">
+        <v>129</v>
+      </c>
+      <c r="X22">
+        <v>106</v>
+      </c>
+      <c r="Y22">
+        <v>870</v>
+      </c>
+      <c r="Z22">
+        <v>25</v>
+      </c>
+      <c r="AA22">
+        <v>38.7</v>
+      </c>
+      <c r="AB22">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="AC22">
+        <v>-97.59999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23">
+        <v>17</v>
+      </c>
+      <c r="E23">
+        <v>417</v>
+      </c>
+      <c r="F23">
+        <v>5829</v>
+      </c>
+      <c r="G23">
+        <v>1068</v>
+      </c>
+      <c r="H23">
+        <v>5.5</v>
+      </c>
+      <c r="I23">
+        <v>12</v>
+      </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
+      <c r="K23">
+        <v>348</v>
+      </c>
+      <c r="L23">
+        <v>346</v>
+      </c>
+      <c r="M23">
+        <v>533</v>
+      </c>
+      <c r="N23">
+        <v>3596</v>
+      </c>
+      <c r="O23">
+        <v>27</v>
+      </c>
+      <c r="P23">
+        <v>7</v>
+      </c>
+      <c r="Q23">
+        <v>6.4</v>
+      </c>
+      <c r="R23">
+        <v>189</v>
+      </c>
+      <c r="S23">
+        <v>507</v>
+      </c>
+      <c r="T23">
+        <v>2233</v>
+      </c>
+      <c r="U23">
+        <v>16</v>
+      </c>
+      <c r="V23">
+        <v>4.4</v>
+      </c>
+      <c r="W23">
+        <v>127</v>
+      </c>
+      <c r="X23">
+        <v>100</v>
+      </c>
+      <c r="Y23">
+        <v>772</v>
+      </c>
+      <c r="Z23">
+        <v>32</v>
+      </c>
+      <c r="AA23">
+        <v>42.8</v>
+      </c>
+      <c r="AB23">
+        <v>5.8</v>
+      </c>
+      <c r="AC23">
+        <v>-133.48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24">
+        <v>17</v>
+      </c>
+      <c r="E24">
+        <v>423</v>
+      </c>
+      <c r="F24">
+        <v>5868</v>
+      </c>
+      <c r="G24">
+        <v>1067</v>
+      </c>
+      <c r="H24">
+        <v>5.5</v>
+      </c>
+      <c r="I24">
+        <v>18</v>
+      </c>
+      <c r="J24">
+        <v>6</v>
+      </c>
+      <c r="K24">
+        <v>347</v>
+      </c>
+      <c r="L24">
+        <v>404</v>
+      </c>
+      <c r="M24">
+        <v>578</v>
+      </c>
+      <c r="N24">
+        <v>3817</v>
+      </c>
+      <c r="O24">
+        <v>34</v>
+      </c>
+      <c r="P24">
+        <v>12</v>
+      </c>
+      <c r="Q24">
+        <v>6.3</v>
+      </c>
+      <c r="R24">
+        <v>200</v>
+      </c>
+      <c r="S24">
+        <v>458</v>
+      </c>
+      <c r="T24">
+        <v>2051</v>
+      </c>
+      <c r="U24">
+        <v>11</v>
+      </c>
+      <c r="V24">
+        <v>4.5</v>
+      </c>
+      <c r="W24">
+        <v>131</v>
+      </c>
+      <c r="X24">
+        <v>122</v>
+      </c>
+      <c r="Y24">
+        <v>964</v>
+      </c>
+      <c r="Z24">
+        <v>16</v>
+      </c>
+      <c r="AA24">
+        <v>43.7</v>
+      </c>
+      <c r="AB24">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="AC24">
+        <v>-85.84999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25">
+        <v>17</v>
+      </c>
+      <c r="E25">
+        <v>427</v>
+      </c>
+      <c r="F25">
+        <v>6140</v>
+      </c>
+      <c r="G25">
+        <v>1112</v>
+      </c>
+      <c r="H25">
+        <v>5.5</v>
+      </c>
+      <c r="I25">
+        <v>25</v>
+      </c>
+      <c r="J25">
+        <v>9</v>
+      </c>
+      <c r="K25">
+        <v>343</v>
+      </c>
+      <c r="L25">
+        <v>378</v>
+      </c>
+      <c r="M25">
+        <v>545</v>
+      </c>
+      <c r="N25">
+        <v>3899</v>
+      </c>
+      <c r="O25">
+        <v>27</v>
+      </c>
+      <c r="P25">
+        <v>16</v>
+      </c>
+      <c r="Q25">
+        <v>6.7</v>
+      </c>
+      <c r="R25">
+        <v>191</v>
+      </c>
+      <c r="S25">
+        <v>531</v>
+      </c>
+      <c r="T25">
+        <v>2241</v>
+      </c>
+      <c r="U25">
+        <v>18</v>
+      </c>
+      <c r="V25">
+        <v>4.2</v>
+      </c>
+      <c r="W25">
+        <v>127</v>
+      </c>
+      <c r="X25">
+        <v>92</v>
+      </c>
+      <c r="Y25">
+        <v>862</v>
+      </c>
+      <c r="Z25">
+        <v>25</v>
+      </c>
+      <c r="AA25">
+        <v>38.3</v>
+      </c>
+      <c r="AB25">
+        <v>12.8</v>
+      </c>
+      <c r="AC25">
+        <v>-73.33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26">
+        <v>17</v>
+      </c>
+      <c r="E26">
+        <v>434</v>
+      </c>
+      <c r="F26">
+        <v>5921</v>
+      </c>
+      <c r="G26">
+        <v>1088</v>
+      </c>
+      <c r="H26">
+        <v>5.4</v>
+      </c>
+      <c r="I26">
+        <v>25</v>
+      </c>
+      <c r="J26">
+        <v>10</v>
+      </c>
+      <c r="K26">
+        <v>361</v>
+      </c>
+      <c r="L26">
+        <v>372</v>
+      </c>
+      <c r="M26">
+        <v>573</v>
+      </c>
+      <c r="N26">
+        <v>3799</v>
+      </c>
+      <c r="O26">
+        <v>30</v>
+      </c>
+      <c r="P26">
+        <v>15</v>
+      </c>
+      <c r="Q26">
+        <v>6.2</v>
+      </c>
+      <c r="R26">
+        <v>192</v>
+      </c>
+      <c r="S26">
+        <v>479</v>
+      </c>
+      <c r="T26">
+        <v>2122</v>
+      </c>
+      <c r="U26">
+        <v>20</v>
+      </c>
+      <c r="V26">
+        <v>4.4</v>
+      </c>
+      <c r="W26">
+        <v>137</v>
+      </c>
+      <c r="X26">
+        <v>101</v>
+      </c>
+      <c r="Y26">
+        <v>826</v>
+      </c>
+      <c r="Z26">
+        <v>32</v>
+      </c>
+      <c r="AA26">
+        <v>39.3</v>
+      </c>
+      <c r="AB26">
+        <v>12.6</v>
+      </c>
+      <c r="AC26">
+        <v>-101.94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27">
+        <v>17</v>
+      </c>
+      <c r="E27">
+        <v>434</v>
+      </c>
+      <c r="F27">
+        <v>5663</v>
+      </c>
+      <c r="G27">
+        <v>1053</v>
+      </c>
+      <c r="H27">
+        <v>5.4</v>
+      </c>
+      <c r="I27">
+        <v>13</v>
+      </c>
+      <c r="J27">
+        <v>3</v>
+      </c>
+      <c r="K27">
+        <v>323</v>
+      </c>
+      <c r="L27">
+        <v>370</v>
+      </c>
+      <c r="M27">
+        <v>561</v>
+      </c>
+      <c r="N27">
+        <v>3676</v>
+      </c>
+      <c r="O27">
+        <v>29</v>
+      </c>
+      <c r="P27">
+        <v>10</v>
+      </c>
+      <c r="Q27">
+        <v>6.1</v>
+      </c>
+      <c r="R27">
+        <v>194</v>
+      </c>
+      <c r="S27">
+        <v>454</v>
+      </c>
+      <c r="T27">
+        <v>1987</v>
+      </c>
+      <c r="U27">
+        <v>14</v>
+      </c>
+      <c r="V27">
+        <v>4.4</v>
+      </c>
+      <c r="W27">
+        <v>102</v>
+      </c>
+      <c r="X27">
+        <v>117</v>
+      </c>
+      <c r="Y27">
+        <v>852</v>
+      </c>
+      <c r="Z27">
+        <v>27</v>
+      </c>
+      <c r="AA27">
+        <v>42.6</v>
+      </c>
+      <c r="AB27">
+        <v>7.1</v>
+      </c>
+      <c r="AC27">
+        <v>-69.33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28">
+        <v>17</v>
+      </c>
+      <c r="E28">
+        <v>435</v>
+      </c>
+      <c r="F28">
+        <v>5816</v>
+      </c>
+      <c r="G28">
+        <v>1040</v>
+      </c>
+      <c r="H28">
+        <v>5.6</v>
+      </c>
+      <c r="I28">
+        <v>12</v>
+      </c>
+      <c r="J28">
+        <v>8</v>
+      </c>
+      <c r="K28">
+        <v>303</v>
+      </c>
+      <c r="L28">
+        <v>316</v>
+      </c>
+      <c r="M28">
+        <v>511</v>
+      </c>
+      <c r="N28">
+        <v>3611</v>
+      </c>
+      <c r="O28">
+        <v>26</v>
+      </c>
+      <c r="P28">
+        <v>4</v>
+      </c>
+      <c r="Q28">
+        <v>6.5</v>
+      </c>
+      <c r="R28">
+        <v>176</v>
+      </c>
+      <c r="S28">
+        <v>488</v>
+      </c>
+      <c r="T28">
+        <v>2205</v>
+      </c>
+      <c r="U28">
+        <v>22</v>
+      </c>
+      <c r="V28">
+        <v>4.5</v>
+      </c>
+      <c r="W28">
+        <v>108</v>
+      </c>
+      <c r="X28">
+        <v>108</v>
+      </c>
+      <c r="Y28">
+        <v>890</v>
+      </c>
+      <c r="Z28">
+        <v>19</v>
+      </c>
+      <c r="AA28">
+        <v>33.3</v>
+      </c>
+      <c r="AB28">
+        <v>5.3</v>
+      </c>
+      <c r="AC28">
+        <v>-61.95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29">
+        <v>17</v>
+      </c>
+      <c r="E29">
+        <v>435</v>
+      </c>
+      <c r="F29">
+        <v>6629</v>
+      </c>
+      <c r="G29">
+        <v>1125</v>
+      </c>
+      <c r="H29">
+        <v>5.9</v>
+      </c>
+      <c r="I29">
+        <v>9</v>
+      </c>
+      <c r="J29">
+        <v>3</v>
+      </c>
+      <c r="K29">
+        <v>389</v>
+      </c>
+      <c r="L29">
+        <v>389</v>
+      </c>
+      <c r="M29">
+        <v>580</v>
+      </c>
+      <c r="N29">
+        <v>4375</v>
+      </c>
+      <c r="O29">
+        <v>29</v>
+      </c>
+      <c r="P29">
+        <v>6</v>
+      </c>
+      <c r="Q29">
+        <v>7.1</v>
+      </c>
+      <c r="R29">
+        <v>219</v>
+      </c>
+      <c r="S29">
+        <v>511</v>
+      </c>
+      <c r="T29">
+        <v>2254</v>
+      </c>
+      <c r="U29">
+        <v>19</v>
+      </c>
+      <c r="V29">
+        <v>4.4</v>
+      </c>
+      <c r="W29">
+        <v>137</v>
+      </c>
+      <c r="X29">
+        <v>105</v>
+      </c>
+      <c r="Y29">
+        <v>808</v>
+      </c>
+      <c r="Z29">
+        <v>33</v>
+      </c>
+      <c r="AA29">
+        <v>45.6</v>
+      </c>
+      <c r="AB29">
+        <v>4.4</v>
+      </c>
+      <c r="AC29">
+        <v>-165.95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30">
+        <v>17</v>
+      </c>
+      <c r="E30">
+        <v>436</v>
+      </c>
+      <c r="F30">
+        <v>5396</v>
+      </c>
+      <c r="G30">
+        <v>1029</v>
+      </c>
+      <c r="H30">
+        <v>5.2</v>
+      </c>
+      <c r="I30">
+        <v>17</v>
+      </c>
+      <c r="J30">
+        <v>6</v>
+      </c>
+      <c r="K30">
+        <v>320</v>
+      </c>
+      <c r="L30">
+        <v>338</v>
+      </c>
+      <c r="M30">
+        <v>516</v>
+      </c>
+      <c r="N30">
+        <v>3278</v>
+      </c>
+      <c r="O30">
+        <v>25</v>
+      </c>
+      <c r="P30">
+        <v>11</v>
+      </c>
+      <c r="Q30">
+        <v>5.9</v>
+      </c>
+      <c r="R30">
+        <v>181</v>
+      </c>
+      <c r="S30">
+        <v>476</v>
+      </c>
+      <c r="T30">
+        <v>2118</v>
+      </c>
+      <c r="U30">
+        <v>24</v>
+      </c>
+      <c r="V30">
+        <v>4.4</v>
+      </c>
+      <c r="W30">
+        <v>118</v>
+      </c>
+      <c r="X30">
+        <v>79</v>
+      </c>
+      <c r="Y30">
+        <v>624</v>
+      </c>
+      <c r="Z30">
+        <v>21</v>
+      </c>
+      <c r="AA30">
+        <v>44.4</v>
+      </c>
+      <c r="AB30">
+        <v>9</v>
+      </c>
+      <c r="AC30">
+        <v>-88.77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:29">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31">
+        <v>17</v>
+      </c>
+      <c r="E31">
+        <v>460</v>
+      </c>
+      <c r="F31">
+        <v>5291</v>
+      </c>
+      <c r="G31">
+        <v>1008</v>
+      </c>
+      <c r="H31">
+        <v>5.2</v>
+      </c>
+      <c r="I31">
+        <v>18</v>
+      </c>
+      <c r="J31">
+        <v>7</v>
+      </c>
+      <c r="K31">
+        <v>314</v>
+      </c>
+      <c r="L31">
+        <v>314</v>
+      </c>
+      <c r="M31">
+        <v>473</v>
+      </c>
+      <c r="N31">
+        <v>3014</v>
+      </c>
+      <c r="O31">
+        <v>27</v>
+      </c>
+      <c r="P31">
+        <v>11</v>
+      </c>
+      <c r="Q31">
+        <v>6</v>
+      </c>
+      <c r="R31">
+        <v>157</v>
+      </c>
+      <c r="S31">
+        <v>503</v>
+      </c>
+      <c r="T31">
+        <v>2277</v>
+      </c>
+      <c r="U31">
+        <v>21</v>
+      </c>
+      <c r="V31">
+        <v>4.5</v>
+      </c>
+      <c r="W31">
+        <v>118</v>
+      </c>
+      <c r="X31">
+        <v>120</v>
+      </c>
+      <c r="Y31">
+        <v>988</v>
+      </c>
+      <c r="Z31">
+        <v>39</v>
+      </c>
+      <c r="AA31">
+        <v>40.4</v>
+      </c>
+      <c r="AB31">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="AC31">
+        <v>-90.11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32">
+        <v>17</v>
+      </c>
+      <c r="E32">
+        <v>468</v>
+      </c>
+      <c r="F32">
+        <v>6039</v>
+      </c>
+      <c r="G32">
+        <v>1046</v>
+      </c>
+      <c r="H32">
+        <v>5.8</v>
+      </c>
+      <c r="I32">
+        <v>22</v>
+      </c>
+      <c r="J32">
+        <v>9</v>
+      </c>
+      <c r="K32">
+        <v>342</v>
+      </c>
+      <c r="L32">
+        <v>349</v>
+      </c>
+      <c r="M32">
+        <v>512</v>
+      </c>
+      <c r="N32">
+        <v>3708</v>
+      </c>
+      <c r="O32">
+        <v>28</v>
+      </c>
+      <c r="P32">
+        <v>13</v>
+      </c>
+      <c r="Q32">
+        <v>6.6</v>
+      </c>
+      <c r="R32">
+        <v>175</v>
+      </c>
+      <c r="S32">
+        <v>482</v>
+      </c>
+      <c r="T32">
+        <v>2331</v>
+      </c>
+      <c r="U32">
+        <v>25</v>
+      </c>
+      <c r="V32">
+        <v>4.8</v>
+      </c>
+      <c r="W32">
+        <v>141</v>
+      </c>
+      <c r="X32">
+        <v>132</v>
+      </c>
+      <c r="Y32">
+        <v>1019</v>
+      </c>
+      <c r="Z32">
+        <v>26</v>
+      </c>
+      <c r="AA32">
+        <v>42.9</v>
+      </c>
+      <c r="AB32">
+        <v>11</v>
+      </c>
+      <c r="AC32">
+        <v>-117.02</v>
+      </c>
+    </row>
+    <row r="33" spans="1:29">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33">
+        <v>17</v>
+      </c>
+      <c r="E33">
+        <v>534</v>
+      </c>
+      <c r="F33">
+        <v>6877</v>
+      </c>
+      <c r="G33">
+        <v>1154</v>
+      </c>
+      <c r="H33">
+        <v>6</v>
+      </c>
+      <c r="I33">
+        <v>17</v>
+      </c>
+      <c r="J33">
+        <v>8</v>
+      </c>
+      <c r="K33">
+        <v>417</v>
+      </c>
+      <c r="L33">
+        <v>360</v>
+      </c>
+      <c r="M33">
+        <v>530</v>
+      </c>
+      <c r="N33">
+        <v>3820</v>
+      </c>
+      <c r="O33">
+        <v>35</v>
+      </c>
+      <c r="P33">
+        <v>9</v>
+      </c>
+      <c r="Q33">
+        <v>6.8</v>
+      </c>
+      <c r="R33">
+        <v>205</v>
+      </c>
+      <c r="S33">
+        <v>592</v>
+      </c>
+      <c r="T33">
+        <v>3057</v>
+      </c>
+      <c r="U33">
+        <v>24</v>
+      </c>
+      <c r="V33">
+        <v>5.2</v>
+      </c>
+      <c r="W33">
+        <v>179</v>
+      </c>
+      <c r="X33">
+        <v>120</v>
+      </c>
+      <c r="Y33">
+        <v>977</v>
+      </c>
+      <c r="Z33">
+        <v>33</v>
+      </c>
+      <c r="AA33">
+        <v>51.4</v>
+      </c>
+      <c r="AB33">
+        <v>8.6</v>
+      </c>
+      <c r="AC33">
+        <v>-220.48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34">
+        <v>389.5</v>
+      </c>
+      <c r="F34">
+        <v>5736.2</v>
+      </c>
+      <c r="G34">
+        <v>1056.6</v>
+      </c>
+      <c r="H34">
+        <v>5.4</v>
+      </c>
+      <c r="I34">
+        <v>20.6</v>
+      </c>
+      <c r="J34">
+        <v>8.5</v>
+      </c>
+      <c r="K34">
+        <v>335.3</v>
+      </c>
+      <c r="L34">
+        <v>363.4</v>
+      </c>
+      <c r="M34">
+        <v>556.6</v>
+      </c>
+      <c r="N34">
+        <v>3699.5</v>
+      </c>
+      <c r="O34">
+        <v>25.3</v>
+      </c>
+      <c r="P34">
+        <v>12.1</v>
+      </c>
+      <c r="Q34">
+        <v>6.2</v>
+      </c>
+      <c r="R34">
+        <v>190.8</v>
+      </c>
+      <c r="S34">
+        <v>459</v>
+      </c>
+      <c r="T34">
+        <v>2036.7</v>
+      </c>
+      <c r="U34">
+        <v>16</v>
+      </c>
+      <c r="V34">
+        <v>4.4</v>
+      </c>
+      <c r="W34">
+        <v>115.1</v>
+      </c>
+      <c r="X34">
+        <v>109.6</v>
+      </c>
+      <c r="Y34">
+        <v>887.9</v>
+      </c>
+      <c r="Z34">
+        <v>29.5</v>
+      </c>
+      <c r="AA34">
+        <v>38.8</v>
+      </c>
+      <c r="AB34">
+        <v>10.7</v>
+      </c>
+      <c r="AC34">
+        <v>-66.7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="C35" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35">
+        <v>12464</v>
+      </c>
+      <c r="F35">
+        <v>183558</v>
+      </c>
+      <c r="G35">
+        <v>33812</v>
+      </c>
+      <c r="H35">
+        <v>5.4</v>
+      </c>
+      <c r="I35">
+        <v>658</v>
+      </c>
+      <c r="J35">
+        <v>271</v>
+      </c>
+      <c r="K35">
+        <v>10730</v>
+      </c>
+      <c r="L35">
+        <v>11629</v>
+      </c>
+      <c r="M35">
+        <v>17811</v>
+      </c>
+      <c r="N35">
+        <v>118384</v>
+      </c>
+      <c r="O35">
+        <v>809</v>
+      </c>
+      <c r="P35">
+        <v>387</v>
+      </c>
+      <c r="Q35">
+        <v>6.2</v>
+      </c>
+      <c r="R35">
+        <v>6104</v>
+      </c>
+      <c r="S35">
+        <v>14687</v>
+      </c>
+      <c r="T35">
+        <v>65174</v>
+      </c>
+      <c r="U35">
+        <v>511</v>
+      </c>
+      <c r="V35">
+        <v>4.4</v>
+      </c>
+      <c r="W35">
+        <v>3682</v>
+      </c>
+      <c r="X35">
+        <v>3506</v>
+      </c>
+      <c r="Y35">
+        <v>28413</v>
+      </c>
+      <c r="Z35">
+        <v>944</v>
+      </c>
+      <c r="AA35">
+        <v>38.8</v>
+      </c>
+      <c r="AB35">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="C36" t="s">
+        <v>94</v>
+      </c>
+      <c r="E36">
+        <v>22.9</v>
+      </c>
+      <c r="F36">
+        <v>337.4</v>
+      </c>
+      <c r="G36">
+        <v>62.2</v>
+      </c>
+      <c r="H36">
+        <v>5.4</v>
+      </c>
+      <c r="I36">
+        <v>1.2</v>
+      </c>
+      <c r="J36">
+        <v>0.5</v>
+      </c>
+      <c r="K36">
+        <v>19.7</v>
+      </c>
+      <c r="L36">
+        <v>21.4</v>
+      </c>
+      <c r="M36">
+        <v>32.7</v>
+      </c>
+      <c r="N36">
+        <v>217.6</v>
+      </c>
+      <c r="O36">
+        <v>1.5</v>
+      </c>
+      <c r="P36">
+        <v>0.7</v>
+      </c>
+      <c r="Q36">
+        <v>6.2</v>
+      </c>
+      <c r="R36">
+        <v>11.2</v>
+      </c>
+      <c r="S36">
+        <v>27</v>
+      </c>
+      <c r="T36">
+        <v>119.8</v>
+      </c>
+      <c r="U36">
+        <v>0.9</v>
+      </c>
+      <c r="V36">
+        <v>4.4</v>
+      </c>
+      <c r="W36">
+        <v>6.8</v>
+      </c>
+      <c r="X36">
+        <v>6.4</v>
+      </c>
+      <c r="Y36">
+        <v>52.2</v>
+      </c>
+      <c r="Z36">
+        <v>1.7</v>
+      </c>
+      <c r="AA36">
+        <v>38.8</v>
+      </c>
+      <c r="AB36">
+        <v>10.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finshed adding the rushing PBI page
</commit_message>
<xml_diff>
--- a/data/NFL_2024_team.xlsx
+++ b/data/NFL_2024_team.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EJTri\Documents\nfl_powerBI\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5397159D-B33C-4613-83BD-4216E9F20213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Offensive_team_stats" sheetId="1" r:id="rId1"/>
     <sheet name="Defensive_team_stats" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1883,8 +1889,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1947,13 +1953,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1991,7 +2005,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2025,6 +2039,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2059,9 +2074,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2234,14 +2250,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2327,7 +2345,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2416,7 +2434,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2505,7 +2523,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2594,7 +2612,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2683,7 +2701,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2772,7 +2790,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2861,7 +2879,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2950,7 +2968,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3039,7 +3057,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3128,7 +3146,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3217,7 +3235,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>12</v>
       </c>
@@ -3306,7 +3324,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>13</v>
       </c>
@@ -3395,7 +3413,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>14</v>
       </c>
@@ -3484,7 +3502,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>15</v>
       </c>
@@ -3573,7 +3591,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>16</v>
       </c>
@@ -3662,7 +3680,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>17</v>
       </c>
@@ -3751,7 +3769,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>18</v>
       </c>
@@ -3840,7 +3858,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>19</v>
       </c>
@@ -3929,7 +3947,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -4018,7 +4036,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -4107,7 +4125,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="22" spans="1:29">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>24</v>
       </c>
@@ -4196,7 +4214,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>25</v>
       </c>
@@ -4285,7 +4303,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="24" spans="1:29">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>26</v>
       </c>
@@ -4374,7 +4392,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="25" spans="1:29">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>27</v>
       </c>
@@ -4463,7 +4481,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="26" spans="1:29">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>28</v>
       </c>
@@ -4552,7 +4570,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="27" spans="1:29">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>29</v>
       </c>
@@ -4641,7 +4659,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="28" spans="1:29">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>30</v>
       </c>
@@ -4730,7 +4748,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="29" spans="1:29">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>31</v>
       </c>
@@ -4819,7 +4837,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="30" spans="1:29">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>32</v>
       </c>
@@ -4908,7 +4926,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="31" spans="1:29">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>33</v>
       </c>
@@ -4997,7 +5015,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="32" spans="1:29">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>34</v>
       </c>
@@ -5086,7 +5104,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="33" spans="1:29">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>35</v>
       </c>
@@ -5175,7 +5193,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="34" spans="1:29">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>36</v>
       </c>
@@ -5261,7 +5279,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="35" spans="1:29">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>37</v>
       </c>
@@ -5344,7 +5362,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="36" spans="1:29">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>38</v>
       </c>
@@ -5433,14 +5451,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5526,7 +5546,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -5615,7 +5635,7 @@
         <v>-12.31</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5665,7 +5685,7 @@
         <v>13</v>
       </c>
       <c r="Q3">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="R3">
         <v>160</v>
@@ -5704,7 +5724,7 @@
         <v>76.38</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -5727,7 +5747,7 @@
         <v>1093</v>
       </c>
       <c r="H4">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I4">
         <v>25</v>
@@ -5793,7 +5813,7 @@
         <v>34.83</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -5858,7 +5878,7 @@
         <v>13</v>
       </c>
       <c r="V5">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="W5">
         <v>112</v>
@@ -5882,7 +5902,7 @@
         <v>-74.11</v>
       </c>
     </row>
-    <row r="6" spans="1:29">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -5947,7 +5967,7 @@
         <v>12</v>
       </c>
       <c r="V6">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="W6">
         <v>83</v>
@@ -5965,13 +5985,13 @@
         <v>31.6</v>
       </c>
       <c r="AB6">
-        <v>16.6</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="AC6">
-        <v>35.95</v>
+        <v>35.950000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -6060,7 +6080,7 @@
         <v>10.82</v>
       </c>
     </row>
-    <row r="8" spans="1:29">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -6149,7 +6169,7 @@
         <v>-58.06</v>
       </c>
     </row>
-    <row r="9" spans="1:29">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -6214,7 +6234,7 @@
         <v>14</v>
       </c>
       <c r="V9">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="W9">
         <v>108</v>
@@ -6238,7 +6258,7 @@
         <v>-34.89</v>
       </c>
     </row>
-    <row r="10" spans="1:29">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -6327,7 +6347,7 @@
         <v>-49.44</v>
       </c>
     </row>
-    <row r="11" spans="1:29">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -6392,7 +6412,7 @@
         <v>12</v>
       </c>
       <c r="V11">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="W11">
         <v>97</v>
@@ -6407,16 +6427,16 @@
         <v>27</v>
       </c>
       <c r="AA11">
-        <v>38.7</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="AB11">
-        <v>8.800000000000001</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="AC11">
         <v>-5.7</v>
       </c>
     </row>
-    <row r="12" spans="1:29">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -6496,7 +6516,7 @@
         <v>30</v>
       </c>
       <c r="AA12">
-        <v>36.3</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="AB12">
         <v>17.5</v>
@@ -6505,7 +6525,7 @@
         <v>-76.45</v>
       </c>
     </row>
-    <row r="13" spans="1:29">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -6570,7 +6590,7 @@
         <v>11</v>
       </c>
       <c r="V13">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="W13">
         <v>107</v>
@@ -6588,13 +6608,13 @@
         <v>34</v>
       </c>
       <c r="AB13">
-        <v>9.300000000000001</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="AC13">
         <v>-11.4</v>
       </c>
     </row>
-    <row r="14" spans="1:29">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -6683,7 +6703,7 @@
         <v>-53.66</v>
       </c>
     </row>
-    <row r="15" spans="1:29">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -6706,7 +6726,7 @@
         <v>1050</v>
       </c>
       <c r="H15">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I15">
         <v>29</v>
@@ -6763,7 +6783,7 @@
         <v>34</v>
       </c>
       <c r="AA15">
-        <v>35.2</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="AB15">
         <v>14</v>
@@ -6772,7 +6792,7 @@
         <v>20.49</v>
       </c>
     </row>
-    <row r="16" spans="1:29">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -6837,7 +6857,7 @@
         <v>18</v>
       </c>
       <c r="V16">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="W16">
         <v>124</v>
@@ -6861,7 +6881,7 @@
         <v>-110.14</v>
       </c>
     </row>
-    <row r="17" spans="1:29">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -6944,13 +6964,13 @@
         <v>40.1</v>
       </c>
       <c r="AB17">
-        <v>8.800000000000001</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="AC17">
         <v>-87.52</v>
       </c>
     </row>
-    <row r="18" spans="1:29">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -7015,7 +7035,7 @@
         <v>13</v>
       </c>
       <c r="V18">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="W18">
         <v>117</v>
@@ -7036,10 +7056,10 @@
         <v>10.6</v>
       </c>
       <c r="AC18">
-        <v>-86.45999999999999</v>
+        <v>-86.46</v>
       </c>
     </row>
-    <row r="19" spans="1:29">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -7122,13 +7142,13 @@
         <v>41.5</v>
       </c>
       <c r="AB19">
-        <v>8.800000000000001</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="AC19">
-        <v>-147.39</v>
+        <v>-147.38999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:29">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -7193,7 +7213,7 @@
         <v>20</v>
       </c>
       <c r="V20">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="W20">
         <v>133</v>
@@ -7208,16 +7228,16 @@
         <v>27</v>
       </c>
       <c r="AA20">
-        <v>39.3</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="AB20">
-        <v>9.300000000000001</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="AC20">
         <v>-107.32</v>
       </c>
     </row>
-    <row r="21" spans="1:29">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -7282,7 +7302,7 @@
         <v>22</v>
       </c>
       <c r="V21">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="W21">
         <v>129</v>
@@ -7303,10 +7323,10 @@
         <v>8.6</v>
       </c>
       <c r="AC21">
-        <v>-93.23999999999999</v>
+        <v>-93.24</v>
       </c>
     </row>
-    <row r="22" spans="1:29">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -7371,7 +7391,7 @@
         <v>18</v>
       </c>
       <c r="V22">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="W22">
         <v>129</v>
@@ -7386,16 +7406,16 @@
         <v>25</v>
       </c>
       <c r="AA22">
-        <v>38.7</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="AB22">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="AC22">
-        <v>-97.59999999999999</v>
+        <v>-97.6</v>
       </c>
     </row>
-    <row r="23" spans="1:29">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -7460,7 +7480,7 @@
         <v>16</v>
       </c>
       <c r="V23">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="W23">
         <v>127</v>
@@ -7481,10 +7501,10 @@
         <v>5.8</v>
       </c>
       <c r="AC23">
-        <v>-133.48</v>
+        <v>-133.47999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:29">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -7567,13 +7587,13 @@
         <v>43.7</v>
       </c>
       <c r="AB24">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="AC24">
-        <v>-85.84999999999999</v>
+        <v>-85.85</v>
       </c>
     </row>
-    <row r="25" spans="1:29">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -7653,7 +7673,7 @@
         <v>25</v>
       </c>
       <c r="AA25">
-        <v>38.3</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="AB25">
         <v>12.8</v>
@@ -7662,7 +7682,7 @@
         <v>-73.33</v>
       </c>
     </row>
-    <row r="26" spans="1:29">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -7727,7 +7747,7 @@
         <v>20</v>
       </c>
       <c r="V26">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="W26">
         <v>137</v>
@@ -7742,7 +7762,7 @@
         <v>32</v>
       </c>
       <c r="AA26">
-        <v>39.3</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="AB26">
         <v>12.6</v>
@@ -7751,7 +7771,7 @@
         <v>-101.94</v>
       </c>
     </row>
-    <row r="27" spans="1:29">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -7816,7 +7836,7 @@
         <v>14</v>
       </c>
       <c r="V27">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="W27">
         <v>102</v>
@@ -7840,7 +7860,7 @@
         <v>-69.33</v>
       </c>
     </row>
-    <row r="28" spans="1:29">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -7920,7 +7940,7 @@
         <v>19</v>
       </c>
       <c r="AA28">
-        <v>33.3</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="AB28">
         <v>5.3</v>
@@ -7929,7 +7949,7 @@
         <v>-61.95</v>
       </c>
     </row>
-    <row r="29" spans="1:29">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -7994,7 +8014,7 @@
         <v>19</v>
       </c>
       <c r="V29">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="W29">
         <v>137</v>
@@ -8012,13 +8032,13 @@
         <v>45.6</v>
       </c>
       <c r="AB29">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="AC29">
         <v>-165.95</v>
       </c>
     </row>
-    <row r="30" spans="1:29">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -8083,7 +8103,7 @@
         <v>24</v>
       </c>
       <c r="V30">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="W30">
         <v>118</v>
@@ -8107,7 +8127,7 @@
         <v>-88.77</v>
       </c>
     </row>
-    <row r="31" spans="1:29">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -8190,13 +8210,13 @@
         <v>40.4</v>
       </c>
       <c r="AB31">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="AC31">
         <v>-90.11</v>
       </c>
     </row>
-    <row r="32" spans="1:29">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -8285,7 +8305,7 @@
         <v>-117.02</v>
       </c>
     </row>
-    <row r="33" spans="1:29">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -8374,7 +8394,7 @@
         <v>-220.48</v>
       </c>
     </row>
-    <row r="34" spans="1:29">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -8388,7 +8408,7 @@
         <v>5736.2</v>
       </c>
       <c r="G34">
-        <v>1056.6</v>
+        <v>1056.5999999999999</v>
       </c>
       <c r="H34">
         <v>5.4</v>
@@ -8433,7 +8453,7 @@
         <v>16</v>
       </c>
       <c r="V34">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="W34">
         <v>115.1</v>
@@ -8448,7 +8468,7 @@
         <v>29.5</v>
       </c>
       <c r="AA34">
-        <v>38.8</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="AB34">
         <v>10.7</v>
@@ -8457,7 +8477,7 @@
         <v>-66.7</v>
       </c>
     </row>
-    <row r="35" spans="1:29">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -8516,7 +8536,7 @@
         <v>511</v>
       </c>
       <c r="V35">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="W35">
         <v>3682</v>
@@ -8531,13 +8551,13 @@
         <v>944</v>
       </c>
       <c r="AA35">
-        <v>38.8</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="AB35">
         <v>10.7</v>
       </c>
     </row>
-    <row r="36" spans="1:29">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -8569,7 +8589,7 @@
         <v>21.4</v>
       </c>
       <c r="M36">
-        <v>32.7</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="N36">
         <v>217.6</v>
@@ -8596,7 +8616,7 @@
         <v>0.9</v>
       </c>
       <c r="V36">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="W36">
         <v>6.8</v>
@@ -8611,7 +8631,7 @@
         <v>1.7</v>
       </c>
       <c r="AA36">
-        <v>38.8</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="AB36">
         <v>10.7</v>

</xml_diff>